<commit_message>
se agregro al mostrar inventario se muestran sus productos
</commit_message>
<xml_diff>
--- a/api/reporte-producto.xlsx
+++ b/api/reporte-producto.xlsx
@@ -61,187 +61,310 @@
     <x:t>Descripción de devolución</x:t>
   </x:si>
   <x:si>
-    <x:t>912ef2ae-20c8-4eb0-7b65-08dc83926143</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Nombre aleatorio</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Descripción aleatoria</x:t>
+    <x:t>ae3212d6-be7a-4eb9-5b29-08dc8cc60340</x:t>
+  </x:si>
+  <x:si>
+    <x:t>RAM AM4 Pro</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Este es un producto en perfecto estado</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Placa madre</x:t>
+  </x:si>
+  <x:si>
+    <x:t>producto aleatorio</x:t>
+  </x:si>
+  <x:si>
+    <x:t>3/06/2024 06:34:13</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Descripcion generica</x:t>
+  </x:si>
+  <x:si>
+    <x:t>ea11181f-f60e-4abb-5b2a-08dc8cc60340</x:t>
+  </x:si>
+  <x:si>
+    <x:t>HDD DDR4 Ultra</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Procesador</x:t>
+  </x:si>
+  <x:si>
+    <x:t>d8f0c798-47c9-42e0-5b2b-08dc8cc60340</x:t>
+  </x:si>
+  <x:si>
+    <x:t>RAM 970 Max</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Fuente de alimentación</x:t>
+  </x:si>
+  <x:si>
+    <x:t>22490b1c-ff10-471f-5b2c-08dc8cc60340</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Mouse 3080 Ultra</x:t>
+  </x:si>
+  <x:si>
+    <x:t>efa150b4-8fb4-4b36-5b2d-08dc8cc60340</x:t>
+  </x:si>
+  <x:si>
+    <x:t>CPU 6800 Extreme</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Memoria RAM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>6c6ac811-0b21-403e-5b2e-08dc8cc60340</x:t>
+  </x:si>
+  <x:si>
+    <x:t>HDD Intel i7 Ultra</x:t>
+  </x:si>
+  <x:si>
+    <x:t>871427c8-1bc6-41f2-5b2f-08dc8cc60340</x:t>
+  </x:si>
+  <x:si>
+    <x:t>CPU DDR4 Expert</x:t>
+  </x:si>
+  <x:si>
+    <x:t>bcda070c-9f92-4328-5b30-08dc8cc60340</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Mouse 500GB Expert</x:t>
+  </x:si>
+  <x:si>
+    <x:t>421794f1-be5f-4bc2-5b31-08dc8cc60340</x:t>
+  </x:si>
+  <x:si>
+    <x:t>RTX 500GB Gaming</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Tarjeta grafica</x:t>
+  </x:si>
+  <x:si>
+    <x:t>a4f927e0-37d9-48d0-5b32-08dc8cc60340</x:t>
+  </x:si>
+  <x:si>
+    <x:t>RX 1TB Master</x:t>
+  </x:si>
+  <x:si>
+    <x:t>15/06/2024 00:18:51</x:t>
+  </x:si>
+  <x:si>
+    <x:t>8605be53-38c4-427b-5b33-08dc8cc60340</x:t>
+  </x:si>
+  <x:si>
+    <x:t>RTX 6800 Turbo</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Disco duro SSD</x:t>
+  </x:si>
+  <x:si>
+    <x:t>728c3b4d-d2e9-460b-5b34-08dc8cc60340</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Placa Madre 970 Turbo</x:t>
+  </x:si>
+  <x:si>
+    <x:t>54155c5f-6c13-440d-5b35-08dc8cc60340</x:t>
+  </x:si>
+  <x:si>
+    <x:t>RX 6800 Plus</x:t>
+  </x:si>
+  <x:si>
+    <x:t>912ffab2-f023-4e2f-5b36-08dc8cc60340</x:t>
+  </x:si>
+  <x:si>
+    <x:t>RX 970 Max</x:t>
+  </x:si>
+  <x:si>
+    <x:t>fe5b9a0e-6bce-4626-5b37-08dc8cc60340</x:t>
+  </x:si>
+  <x:si>
+    <x:t>RAM 6800 Max</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1313ff96-dee1-485b-5b38-08dc8cc60340</x:t>
+  </x:si>
+  <x:si>
+    <x:t>RAM 970 Turbo</x:t>
+  </x:si>
+  <x:si>
+    <x:t>0dc01bd6-8910-465d-5b39-08dc8cc60340</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Placa Madre 144Hz Turbo</x:t>
   </x:si>
   <x:si>
     <x:t>Tarjeta gráfica</x:t>
   </x:si>
   <x:si>
-    <x:t>producto aleatorio</x:t>
-  </x:si>
-  <x:si>
-    <x:t>3/06/2024 06:34:13</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Descripcion generica</x:t>
-  </x:si>
-  <x:si>
-    <x:t>3/06/2024 07:27:30</x:t>
-  </x:si>
-  <x:si>
-    <x:t>97b93926-77fd-43c4-7b66-08dc83926143</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Fuente de alimentación</x:t>
-  </x:si>
-  <x:si>
-    <x:t>c335275f-3ac2-4b1d-7b67-08dc83926143</x:t>
-  </x:si>
-  <x:si>
-    <x:t>b7538d2b-b7e0-418d-7b68-08dc83926143</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Disco duro SSD</x:t>
-  </x:si>
-  <x:si>
-    <x:t>916a2e0e-ae2d-424f-7b69-08dc83926143</x:t>
-  </x:si>
-  <x:si>
-    <x:t>1f748452-3b6f-4479-7b6a-08dc83926143</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Memoria RAM</x:t>
-  </x:si>
-  <x:si>
-    <x:t>01aecce8-f71c-42ab-7b6b-08dc83926143</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Procesador</x:t>
-  </x:si>
-  <x:si>
-    <x:t>a08f9ad1-2bef-4f06-7b6c-08dc83926143</x:t>
-  </x:si>
-  <x:si>
-    <x:t>1401d521-d96e-4ba9-7b6d-08dc83926143</x:t>
-  </x:si>
-  <x:si>
-    <x:t>2a306655-89a8-4405-7b6e-08dc83926143</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Tarjeta grafica</x:t>
-  </x:si>
-  <x:si>
-    <x:t>103f5722-0ed9-46d4-7b6f-08dc83926143</x:t>
-  </x:si>
-  <x:si>
-    <x:t>4962d04e-7789-4734-7b70-08dc83926143</x:t>
-  </x:si>
-  <x:si>
-    <x:t>f439e2db-3898-4ef3-7b71-08dc83926143</x:t>
-  </x:si>
-  <x:si>
-    <x:t>f760d08a-f2ad-4500-7b72-08dc83926143</x:t>
-  </x:si>
-  <x:si>
-    <x:t>9c672064-6dee-4742-7b73-08dc83926143</x:t>
-  </x:si>
-  <x:si>
-    <x:t>601a75dc-706c-49c7-7b74-08dc83926143</x:t>
-  </x:si>
-  <x:si>
-    <x:t>5b5c4766-c2c0-4ccc-7b75-08dc83926143</x:t>
-  </x:si>
-  <x:si>
-    <x:t>304cf75b-0603-4a9f-7b76-08dc83926143</x:t>
-  </x:si>
-  <x:si>
-    <x:t>58d3c904-c004-4c4c-7b77-08dc83926143</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Placa madre</x:t>
-  </x:si>
-  <x:si>
-    <x:t>fb22bde0-2643-4d3c-7b78-08dc83926143</x:t>
-  </x:si>
-  <x:si>
-    <x:t>840f47d9-8cc8-4739-7b79-08dc83926143</x:t>
-  </x:si>
-  <x:si>
-    <x:t>f2433e76-1713-42fa-7b7a-08dc83926143</x:t>
-  </x:si>
-  <x:si>
-    <x:t>1e9f137e-e89c-4bd3-7b7b-08dc83926143</x:t>
-  </x:si>
-  <x:si>
-    <x:t>ab5408e5-0779-4b63-7b7c-08dc83926143</x:t>
-  </x:si>
-  <x:si>
-    <x:t>bea165e2-9043-41d7-7b7d-08dc83926143</x:t>
-  </x:si>
-  <x:si>
-    <x:t>7412b700-d8c9-44c9-7b7e-08dc83926143</x:t>
-  </x:si>
-  <x:si>
-    <x:t>91b7df88-d171-425b-7b7f-08dc83926143</x:t>
-  </x:si>
-  <x:si>
-    <x:t>0ae7908c-27d0-439a-7b80-08dc83926143</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Tecnologia de la nueva</x:t>
-  </x:si>
-  <x:si>
-    <x:t>16/04/2024 00:00:00</x:t>
-  </x:si>
-  <x:si>
-    <x:t>5d2ffd0a-ba68-44e9-7b81-08dc83926143</x:t>
-  </x:si>
-  <x:si>
-    <x:t>ce44a197-fca1-4ab5-7b82-08dc83926143</x:t>
-  </x:si>
-  <x:si>
-    <x:t>9b49ec6b-abb1-4450-7b83-08dc83926143</x:t>
-  </x:si>
-  <x:si>
-    <x:t>30dcfe93-37c0-43a2-7b84-08dc83926143</x:t>
-  </x:si>
-  <x:si>
-    <x:t>7bf7e358-1f43-4807-7b85-08dc83926143</x:t>
-  </x:si>
-  <x:si>
-    <x:t>cdca8149-5b5a-4efe-7b86-08dc83926143</x:t>
-  </x:si>
-  <x:si>
-    <x:t>34185879-ea90-4e87-7b87-08dc83926143</x:t>
-  </x:si>
-  <x:si>
-    <x:t>854e1031-6fa6-4790-7b88-08dc83926143</x:t>
-  </x:si>
-  <x:si>
-    <x:t>d0e0a1f4-6ddc-4fd2-7b89-08dc83926143</x:t>
-  </x:si>
-  <x:si>
-    <x:t>e6f6432d-96cd-4fbf-7b8a-08dc83926143</x:t>
-  </x:si>
-  <x:si>
-    <x:t>b4a7eab1-cb64-42b6-7b8b-08dc83926143</x:t>
-  </x:si>
-  <x:si>
-    <x:t>017beaf3-ea01-4421-7b8c-08dc83926143</x:t>
-  </x:si>
-  <x:si>
-    <x:t>16bd2e39-ee24-4447-7b8d-08dc83926143</x:t>
-  </x:si>
-  <x:si>
-    <x:t>a9d7dd3d-5bc0-4d72-7b8e-08dc83926143</x:t>
-  </x:si>
-  <x:si>
-    <x:t>9b9e318f-4363-465e-7b8f-08dc83926143</x:t>
-  </x:si>
-  <x:si>
-    <x:t>24134090-1de1-4786-7b90-08dc83926143</x:t>
-  </x:si>
-  <x:si>
-    <x:t>d9f2be38-1bc4-49ab-7b91-08dc83926143</x:t>
-  </x:si>
-  <x:si>
-    <x:t>858fe0c3-72a7-4ffd-7b92-08dc83926143</x:t>
+    <x:t>536bd520-7639-40b6-5b3a-08dc8cc60340</x:t>
+  </x:si>
+  <x:si>
+    <x:t>HDD 1TB Extreme</x:t>
+  </x:si>
+  <x:si>
+    <x:t>53fa2300-0281-48b4-5b3b-08dc8cc60340</x:t>
+  </x:si>
+  <x:si>
+    <x:t>RTX AM4 Elite</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1398d62b-bd9a-4a1f-5b3c-08dc8cc60340</x:t>
+  </x:si>
+  <x:si>
+    <x:t>RAM 3080 Pro</x:t>
+  </x:si>
+  <x:si>
+    <x:t>7f22c92d-957f-469d-5b3d-08dc8cc60340</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Monitor 970 Prime</x:t>
+  </x:si>
+  <x:si>
+    <x:t>b40e2458-f817-4ca7-5b3e-08dc8cc60340</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Mouse DDR4 Prime</x:t>
+  </x:si>
+  <x:si>
+    <x:t>19570505-2ed2-4da4-5b3f-08dc8cc60340</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Monitor 500GB Extreme</x:t>
+  </x:si>
+  <x:si>
+    <x:t>85cca03c-14b5-46dd-5b40-08dc8cc60340</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Fuente DDR4 Pro</x:t>
+  </x:si>
+  <x:si>
+    <x:t>beeca787-1ef2-47b5-5b41-08dc8cc60340</x:t>
+  </x:si>
+  <x:si>
+    <x:t>HDD 6800 Extreme</x:t>
+  </x:si>
+  <x:si>
+    <x:t>551beb0e-3f1e-4e31-5b42-08dc8cc60340</x:t>
+  </x:si>
+  <x:si>
+    <x:t>RX Óptico Turbo</x:t>
+  </x:si>
+  <x:si>
+    <x:t>42d71852-9a62-4c25-5b43-08dc8cc60340</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Placa Madre Óptico Advanced</x:t>
+  </x:si>
+  <x:si>
+    <x:t>df83208c-75b7-4086-5b44-08dc8cc60340</x:t>
+  </x:si>
+  <x:si>
+    <x:t>CPU Óptico Expert</x:t>
+  </x:si>
+  <x:si>
+    <x:t>862ee065-c74f-414e-5b45-08dc8cc60340</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Mouse 3080 Pro</x:t>
+  </x:si>
+  <x:si>
+    <x:t>5bca5869-e14f-4a17-5b46-08dc8cc60340</x:t>
+  </x:si>
+  <x:si>
+    <x:t>GTX Óptico Advanced</x:t>
+  </x:si>
+  <x:si>
+    <x:t>efa122cd-301b-4e4c-5b47-08dc8cc60340</x:t>
+  </x:si>
+  <x:si>
+    <x:t>RTX 6800 Elite</x:t>
+  </x:si>
+  <x:si>
+    <x:t>97536079-73e8-4abe-5b48-08dc8cc60340</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Mouse 3080 Turbo</x:t>
+  </x:si>
+  <x:si>
+    <x:t>e66d51e8-4cbf-48af-5b49-08dc8cc60340</x:t>
+  </x:si>
+  <x:si>
+    <x:t>HDD 750W Gaming</x:t>
+  </x:si>
+  <x:si>
+    <x:t>87253bc1-c03f-44f8-5b4a-08dc8cc60340</x:t>
+  </x:si>
+  <x:si>
+    <x:t>GPU AM4 Elite</x:t>
+  </x:si>
+  <x:si>
+    <x:t>30e78dc3-f1c3-4a34-5b4b-08dc8cc60340</x:t>
+  </x:si>
+  <x:si>
+    <x:t>GPU Óptico Turbo</x:t>
+  </x:si>
+  <x:si>
+    <x:t>b6d20516-9509-4845-5b4c-08dc8cc60340</x:t>
+  </x:si>
+  <x:si>
+    <x:t>GPU 500GB Expert</x:t>
+  </x:si>
+  <x:si>
+    <x:t>c26a0578-adc3-4ecd-5b4d-08dc8cc60340</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Teclado 500GB Gaming</x:t>
+  </x:si>
+  <x:si>
+    <x:t>c6fc0e89-4fbe-4df2-5b4e-08dc8cc60340</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Mouse 750W Prime</x:t>
+  </x:si>
+  <x:si>
+    <x:t>219fc855-3c9a-4deb-5b4f-08dc8cc60340</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Fuente AM4 Prime</x:t>
+  </x:si>
+  <x:si>
+    <x:t>271ad3ea-ab7c-47ad-5b50-08dc8cc60340</x:t>
+  </x:si>
+  <x:si>
+    <x:t>RAM DDR4 Turbo</x:t>
+  </x:si>
+  <x:si>
+    <x:t>8b34de23-c1d5-493f-5b51-08dc8cc60340</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Placa Madre AM4 Ultra</x:t>
+  </x:si>
+  <x:si>
+    <x:t>46a8fa95-b13a-4c5b-5b52-08dc8cc60340</x:t>
+  </x:si>
+  <x:si>
+    <x:t>HDD DDR4 Expert</x:t>
+  </x:si>
+  <x:si>
+    <x:t>b5a7c5c8-8b3c-46b7-5b53-08dc8cc60340</x:t>
+  </x:si>
+  <x:si>
+    <x:t>SSD Ryzen 5 Prime</x:t>
+  </x:si>
+  <x:si>
+    <x:t>5ea1d5ad-c17b-44bf-5b54-08dc8cc60340</x:t>
+  </x:si>
+  <x:si>
+    <x:t>RTX 970 Extreme</x:t>
+  </x:si>
+  <x:si>
+    <x:t>89e9c026-368c-4cf3-5b55-08dc8cc60340</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Monitor 500GB Expert</x:t>
   </x:si>
   <x:si>
     <x:t>Importaciones SA</x:t>
@@ -250,43 +373,34 @@
     <x:t>26/05/2024 00:00:00</x:t>
   </x:si>
   <x:si>
-    <x:t>f9b5765b-f966-4d86-7b93-08dc83926143</x:t>
-  </x:si>
-  <x:si>
-    <x:t>8f3d71b2-055f-47c4-7b94-08dc83926143</x:t>
-  </x:si>
-  <x:si>
-    <x:t>09d73bcb-09af-45fc-7b95-08dc83926143</x:t>
-  </x:si>
-  <x:si>
-    <x:t>57fa9965-b0fa-4130-7b96-08dc83926143</x:t>
-  </x:si>
-  <x:si>
-    <x:t>d742ec77-c321-4caf-9a01-a60affcbb407</x:t>
-  </x:si>
-  <x:si>
-    <x:t>A520M-K</x:t>
-  </x:si>
-  <x:si>
-    <x:t>PRIME A520M-K Mainboard</x:t>
-  </x:si>
-  <x:si>
-    <x:t>30/05/2024 23:49:07</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Placas madre modelo  PRIME A520M-K</x:t>
-  </x:si>
-  <x:si>
-    <x:t>3fbf76aa-6385-4478-902d-c7e9f73df546</x:t>
-  </x:si>
-  <x:si>
-    <x:t>placa asus</x:t>
-  </x:si>
-  <x:si>
-    <x:t>placa marca asus</x:t>
-  </x:si>
-  <x:si>
-    <x:t>30/05/2024 21:49:59</x:t>
+    <x:t>382e61bb-c871-48e7-5b56-08dc8cc60340</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Fuente 144Hz Master</x:t>
+  </x:si>
+  <x:si>
+    <x:t>66db2a82-43a7-432a-5b57-08dc8cc60340</x:t>
+  </x:si>
+  <x:si>
+    <x:t>RX Óptico Master</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1797eb92-546a-41e9-5b58-08dc8cc60340</x:t>
+  </x:si>
+  <x:si>
+    <x:t>RX 6800 Expert</x:t>
+  </x:si>
+  <x:si>
+    <x:t>fe470402-0634-439f-5b59-08dc8cc60340</x:t>
+  </x:si>
+  <x:si>
+    <x:t>SSD Óptico Extreme</x:t>
+  </x:si>
+  <x:si>
+    <x:t>8ae09d9b-0247-4397-5b5a-08dc8cc60340</x:t>
+  </x:si>
+  <x:si>
+    <x:t>GTX 750W Plus</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -350,8 +464,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<x:table xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Reportedeproductos" displayName="Reportedeproductos" ref="A1:O53" totalsRowShown="0">
-  <x:autoFilter ref="A1:O53"/>
+<x:table xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Reportedeproductos" displayName="Reportedeproductos" ref="A1:O51" totalsRowShown="0">
+  <x:autoFilter ref="A1:O51"/>
   <x:tableColumns count="15">
     <x:tableColumn id="1" name="ID"/>
     <x:tableColumn id="2" name="Nombre del producto"/>
@@ -661,7 +775,7 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:O53"/>
+  <x:dimension ref="A1:O51"/>
   <x:sheetViews>
     <x:sheetView workbookViewId="0"/>
   </x:sheetViews>
@@ -725,16 +839,16 @@
         <x:v>17</x:v>
       </x:c>
       <x:c r="D2" s="0">
-        <x:v>214</x:v>
+        <x:v>473</x:v>
       </x:c>
       <x:c r="E2" s="0">
-        <x:v>86.74</x:v>
+        <x:v>5.5498</x:v>
       </x:c>
       <x:c r="G2" s="0" t="s">
         <x:v>18</x:v>
       </x:c>
       <x:c r="H2" s="0">
-        <x:v>24113.72</x:v>
+        <x:v>27.749</x:v>
       </x:c>
       <x:c r="I2" s="0" t="s">
         <x:v>19</x:v>
@@ -746,39 +860,42 @@
         <x:v>21</x:v>
       </x:c>
       <x:c r="L2" s="0">
-        <x:v>278</x:v>
-      </x:c>
-      <x:c r="M2" s="0">
-        <x:v>9</x:v>
-      </x:c>
-      <x:c r="N2" s="0" t="s">
-        <x:v>22</x:v>
-      </x:c>
-      <x:c r="O2" s="0" t="s">
-        <x:v>21</x:v>
+        <x:v>5</x:v>
       </x:c>
     </x:row>
     <x:row r="3" spans="1:15">
       <x:c r="A3" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="B3" s="0" t="s">
         <x:v>23</x:v>
       </x:c>
-      <x:c r="B3" s="0" t="s">
-        <x:v>16</x:v>
-      </x:c>
       <x:c r="C3" s="0" t="s">
         <x:v>17</x:v>
       </x:c>
+      <x:c r="D3" s="0">
+        <x:v>473</x:v>
+      </x:c>
       <x:c r="E3" s="0">
-        <x:v>61.1797</x:v>
+        <x:v>84.0028</x:v>
       </x:c>
       <x:c r="G3" s="0" t="s">
         <x:v>24</x:v>
       </x:c>
       <x:c r="H3" s="0">
-        <x:v>0</x:v>
+        <x:v>41665.3888</x:v>
+      </x:c>
+      <x:c r="I3" s="0" t="s">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="J3" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="K3" s="0" t="s">
+        <x:v>21</x:v>
       </x:c>
       <x:c r="L3" s="0">
-        <x:v>0</x:v>
+        <x:v>496</x:v>
       </x:c>
     </x:row>
     <x:row r="4" spans="1:15">
@@ -786,22 +903,22 @@
         <x:v>25</x:v>
       </x:c>
       <x:c r="B4" s="0" t="s">
-        <x:v>16</x:v>
+        <x:v>26</x:v>
       </x:c>
       <x:c r="C4" s="0" t="s">
         <x:v>17</x:v>
       </x:c>
       <x:c r="D4" s="0">
-        <x:v>214</x:v>
+        <x:v>473</x:v>
       </x:c>
       <x:c r="E4" s="0">
-        <x:v>48.0318</x:v>
+        <x:v>5.7977</x:v>
       </x:c>
       <x:c r="G4" s="0" t="s">
-        <x:v>18</x:v>
+        <x:v>27</x:v>
       </x:c>
       <x:c r="H4" s="0">
-        <x:v>21422.1828</x:v>
+        <x:v>2817.6822</x:v>
       </x:c>
       <x:c r="I4" s="0" t="s">
         <x:v>19</x:v>
@@ -813,125 +930,149 @@
         <x:v>21</x:v>
       </x:c>
       <x:c r="L4" s="0">
-        <x:v>446</x:v>
+        <x:v>486</x:v>
       </x:c>
     </x:row>
     <x:row r="5" spans="1:15">
       <x:c r="A5" s="0" t="s">
-        <x:v>26</x:v>
+        <x:v>28</x:v>
       </x:c>
       <x:c r="B5" s="0" t="s">
-        <x:v>16</x:v>
+        <x:v>29</x:v>
       </x:c>
       <x:c r="C5" s="0" t="s">
         <x:v>17</x:v>
       </x:c>
-      <x:c r="D5" s="0">
-        <x:v>214</x:v>
-      </x:c>
       <x:c r="E5" s="0">
-        <x:v>86.8961</x:v>
+        <x:v>53.8384</x:v>
       </x:c>
       <x:c r="G5" s="0" t="s">
-        <x:v>27</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="H5" s="0">
-        <x:v>38408.0762</x:v>
-      </x:c>
-      <x:c r="I5" s="0" t="s">
-        <x:v>19</x:v>
-      </x:c>
-      <x:c r="J5" s="0" t="s">
-        <x:v>20</x:v>
-      </x:c>
-      <x:c r="K5" s="0" t="s">
-        <x:v>21</x:v>
+        <x:v>0</x:v>
       </x:c>
       <x:c r="L5" s="0">
-        <x:v>442</x:v>
+        <x:v>0</x:v>
       </x:c>
     </x:row>
     <x:row r="6" spans="1:15">
       <x:c r="A6" s="0" t="s">
-        <x:v>28</x:v>
+        <x:v>30</x:v>
       </x:c>
       <x:c r="B6" s="0" t="s">
-        <x:v>16</x:v>
+        <x:v>31</x:v>
       </x:c>
       <x:c r="C6" s="0" t="s">
         <x:v>17</x:v>
       </x:c>
+      <x:c r="D6" s="0">
+        <x:v>473</x:v>
+      </x:c>
       <x:c r="E6" s="0">
-        <x:v>88.3364</x:v>
+        <x:v>55.5929</x:v>
       </x:c>
       <x:c r="G6" s="0" t="s">
-        <x:v>18</x:v>
+        <x:v>32</x:v>
       </x:c>
       <x:c r="H6" s="0">
-        <x:v>0</x:v>
+        <x:v>6671.148</x:v>
+      </x:c>
+      <x:c r="I6" s="0" t="s">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="J6" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="K6" s="0" t="s">
+        <x:v>21</x:v>
       </x:c>
       <x:c r="L6" s="0">
-        <x:v>0</x:v>
+        <x:v>120</x:v>
       </x:c>
     </x:row>
     <x:row r="7" spans="1:15">
       <x:c r="A7" s="0" t="s">
-        <x:v>29</x:v>
+        <x:v>33</x:v>
       </x:c>
       <x:c r="B7" s="0" t="s">
-        <x:v>16</x:v>
+        <x:v>34</x:v>
       </x:c>
       <x:c r="C7" s="0" t="s">
         <x:v>17</x:v>
       </x:c>
+      <x:c r="D7" s="0">
+        <x:v>473</x:v>
+      </x:c>
       <x:c r="E7" s="0">
-        <x:v>0.5325</x:v>
+        <x:v>66.9699</x:v>
       </x:c>
       <x:c r="G7" s="0" t="s">
-        <x:v>30</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="H7" s="0">
-        <x:v>0</x:v>
+        <x:v>24912.8028</x:v>
+      </x:c>
+      <x:c r="I7" s="0" t="s">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="J7" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="K7" s="0" t="s">
+        <x:v>21</x:v>
       </x:c>
       <x:c r="L7" s="0">
-        <x:v>0</x:v>
+        <x:v>372</x:v>
       </x:c>
     </x:row>
     <x:row r="8" spans="1:15">
       <x:c r="A8" s="0" t="s">
-        <x:v>31</x:v>
+        <x:v>35</x:v>
       </x:c>
       <x:c r="B8" s="0" t="s">
-        <x:v>16</x:v>
+        <x:v>36</x:v>
       </x:c>
       <x:c r="C8" s="0" t="s">
         <x:v>17</x:v>
       </x:c>
+      <x:c r="D8" s="0">
+        <x:v>473</x:v>
+      </x:c>
       <x:c r="E8" s="0">
-        <x:v>8.9013</x:v>
+        <x:v>81.0468</x:v>
       </x:c>
       <x:c r="G8" s="0" t="s">
-        <x:v>32</x:v>
+        <x:v>18</x:v>
       </x:c>
       <x:c r="H8" s="0">
-        <x:v>0</x:v>
+        <x:v>13048.5348</x:v>
+      </x:c>
+      <x:c r="I8" s="0" t="s">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="J8" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="K8" s="0" t="s">
+        <x:v>21</x:v>
       </x:c>
       <x:c r="L8" s="0">
-        <x:v>0</x:v>
+        <x:v>161</x:v>
       </x:c>
     </x:row>
     <x:row r="9" spans="1:15">
       <x:c r="A9" s="0" t="s">
-        <x:v>33</x:v>
+        <x:v>37</x:v>
       </x:c>
       <x:c r="B9" s="0" t="s">
-        <x:v>16</x:v>
+        <x:v>38</x:v>
       </x:c>
       <x:c r="C9" s="0" t="s">
         <x:v>17</x:v>
       </x:c>
       <x:c r="E9" s="0">
-        <x:v>74.2483</x:v>
+        <x:v>4.3259</x:v>
       </x:c>
       <x:c r="G9" s="0" t="s">
         <x:v>24</x:v>
@@ -945,48 +1086,60 @@
     </x:row>
     <x:row r="10" spans="1:15">
       <x:c r="A10" s="0" t="s">
-        <x:v>34</x:v>
+        <x:v>39</x:v>
       </x:c>
       <x:c r="B10" s="0" t="s">
-        <x:v>16</x:v>
+        <x:v>40</x:v>
       </x:c>
       <x:c r="C10" s="0" t="s">
         <x:v>17</x:v>
       </x:c>
+      <x:c r="D10" s="0">
+        <x:v>473</x:v>
+      </x:c>
       <x:c r="E10" s="0">
-        <x:v>43.6009</x:v>
+        <x:v>5.9406</x:v>
       </x:c>
       <x:c r="G10" s="0" t="s">
-        <x:v>27</x:v>
+        <x:v>41</x:v>
       </x:c>
       <x:c r="H10" s="0">
-        <x:v>0</x:v>
+        <x:v>2281.1904</x:v>
+      </x:c>
+      <x:c r="I10" s="0" t="s">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="J10" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="K10" s="0" t="s">
+        <x:v>21</x:v>
       </x:c>
       <x:c r="L10" s="0">
-        <x:v>0</x:v>
+        <x:v>384</x:v>
       </x:c>
     </x:row>
     <x:row r="11" spans="1:15">
       <x:c r="A11" s="0" t="s">
-        <x:v>35</x:v>
+        <x:v>42</x:v>
       </x:c>
       <x:c r="B11" s="0" t="s">
-        <x:v>16</x:v>
+        <x:v>43</x:v>
       </x:c>
       <x:c r="C11" s="0" t="s">
         <x:v>17</x:v>
       </x:c>
       <x:c r="D11" s="0">
-        <x:v>214</x:v>
+        <x:v>473</x:v>
       </x:c>
       <x:c r="E11" s="0">
-        <x:v>76.3704</x:v>
+        <x:v>35.7158</x:v>
       </x:c>
       <x:c r="G11" s="0" t="s">
-        <x:v>36</x:v>
+        <x:v>32</x:v>
       </x:c>
       <x:c r="H11" s="0">
-        <x:v>22071.0456</x:v>
+        <x:v>4285.896</x:v>
       </x:c>
       <x:c r="I11" s="0" t="s">
         <x:v>19</x:v>
@@ -998,13 +1151,13 @@
         <x:v>21</x:v>
       </x:c>
       <x:c r="L11" s="0">
-        <x:v>289</x:v>
+        <x:v>120</x:v>
       </x:c>
       <x:c r="M11" s="0">
-        <x:v>3</x:v>
+        <x:v>1</x:v>
       </x:c>
       <x:c r="N11" s="0" t="s">
-        <x:v>22</x:v>
+        <x:v>44</x:v>
       </x:c>
       <x:c r="O11" s="0" t="s">
         <x:v>21</x:v>
@@ -1012,48 +1165,60 @@
     </x:row>
     <x:row r="12" spans="1:15">
       <x:c r="A12" s="0" t="s">
-        <x:v>37</x:v>
+        <x:v>45</x:v>
       </x:c>
       <x:c r="B12" s="0" t="s">
-        <x:v>16</x:v>
+        <x:v>46</x:v>
       </x:c>
       <x:c r="C12" s="0" t="s">
         <x:v>17</x:v>
       </x:c>
+      <x:c r="D12" s="0">
+        <x:v>473</x:v>
+      </x:c>
       <x:c r="E12" s="0">
-        <x:v>79.6158</x:v>
+        <x:v>70.8502</x:v>
       </x:c>
       <x:c r="G12" s="0" t="s">
-        <x:v>36</x:v>
+        <x:v>47</x:v>
       </x:c>
       <x:c r="H12" s="0">
-        <x:v>0</x:v>
+        <x:v>17641.6998</x:v>
+      </x:c>
+      <x:c r="I12" s="0" t="s">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="J12" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="K12" s="0" t="s">
+        <x:v>21</x:v>
       </x:c>
       <x:c r="L12" s="0">
-        <x:v>0</x:v>
+        <x:v>249</x:v>
       </x:c>
     </x:row>
     <x:row r="13" spans="1:15">
       <x:c r="A13" s="0" t="s">
-        <x:v>38</x:v>
+        <x:v>48</x:v>
       </x:c>
       <x:c r="B13" s="0" t="s">
-        <x:v>16</x:v>
+        <x:v>49</x:v>
       </x:c>
       <x:c r="C13" s="0" t="s">
         <x:v>17</x:v>
       </x:c>
       <x:c r="D13" s="0">
-        <x:v>214</x:v>
+        <x:v>473</x:v>
       </x:c>
       <x:c r="E13" s="0">
-        <x:v>78.1186</x:v>
+        <x:v>21.4565</x:v>
       </x:c>
       <x:c r="G13" s="0" t="s">
-        <x:v>30</x:v>
+        <x:v>27</x:v>
       </x:c>
       <x:c r="H13" s="0">
-        <x:v>34528.4212</x:v>
+        <x:v>10642.424</x:v>
       </x:c>
       <x:c r="I13" s="0" t="s">
         <x:v>19</x:v>
@@ -1065,62 +1230,65 @@
         <x:v>21</x:v>
       </x:c>
       <x:c r="L13" s="0">
-        <x:v>442</x:v>
+        <x:v>496</x:v>
       </x:c>
     </x:row>
     <x:row r="14" spans="1:15">
       <x:c r="A14" s="0" t="s">
-        <x:v>39</x:v>
+        <x:v>50</x:v>
       </x:c>
       <x:c r="B14" s="0" t="s">
-        <x:v>16</x:v>
+        <x:v>51</x:v>
       </x:c>
       <x:c r="C14" s="0" t="s">
         <x:v>17</x:v>
       </x:c>
+      <x:c r="D14" s="0">
+        <x:v>473</x:v>
+      </x:c>
       <x:c r="E14" s="0">
-        <x:v>2.6486</x:v>
+        <x:v>90.5104</x:v>
       </x:c>
       <x:c r="G14" s="0" t="s">
-        <x:v>36</x:v>
+        <x:v>18</x:v>
       </x:c>
       <x:c r="H14" s="0">
-        <x:v>0</x:v>
+        <x:v>42087.336</x:v>
+      </x:c>
+      <x:c r="I14" s="0" t="s">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="J14" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="K14" s="0" t="s">
+        <x:v>21</x:v>
       </x:c>
       <x:c r="L14" s="0">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="M14" s="0">
-        <x:v>8</x:v>
-      </x:c>
-      <x:c r="N14" s="0" t="s">
-        <x:v>22</x:v>
-      </x:c>
-      <x:c r="O14" s="0" t="s">
-        <x:v>21</x:v>
+        <x:v>465</x:v>
       </x:c>
     </x:row>
     <x:row r="15" spans="1:15">
       <x:c r="A15" s="0" t="s">
-        <x:v>40</x:v>
+        <x:v>52</x:v>
       </x:c>
       <x:c r="B15" s="0" t="s">
-        <x:v>16</x:v>
+        <x:v>53</x:v>
       </x:c>
       <x:c r="C15" s="0" t="s">
         <x:v>17</x:v>
       </x:c>
       <x:c r="D15" s="0">
-        <x:v>214</x:v>
+        <x:v>473</x:v>
       </x:c>
       <x:c r="E15" s="0">
-        <x:v>75.6908</x:v>
+        <x:v>46.9208</x:v>
       </x:c>
       <x:c r="G15" s="0" t="s">
-        <x:v>36</x:v>
+        <x:v>18</x:v>
       </x:c>
       <x:c r="H15" s="0">
-        <x:v>29140.958</x:v>
+        <x:v>6521.9912</x:v>
       </x:c>
       <x:c r="I15" s="0" t="s">
         <x:v>19</x:v>
@@ -1132,53 +1300,74 @@
         <x:v>21</x:v>
       </x:c>
       <x:c r="L15" s="0">
-        <x:v>385</x:v>
+        <x:v>139</x:v>
+      </x:c>
+      <x:c r="M15" s="0">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="N15" s="0" t="s">
+        <x:v>44</x:v>
+      </x:c>
+      <x:c r="O15" s="0" t="s">
+        <x:v>21</x:v>
       </x:c>
     </x:row>
     <x:row r="16" spans="1:15">
       <x:c r="A16" s="0" t="s">
-        <x:v>41</x:v>
+        <x:v>54</x:v>
       </x:c>
       <x:c r="B16" s="0" t="s">
-        <x:v>16</x:v>
+        <x:v>55</x:v>
       </x:c>
       <x:c r="C16" s="0" t="s">
         <x:v>17</x:v>
       </x:c>
+      <x:c r="D16" s="0">
+        <x:v>473</x:v>
+      </x:c>
       <x:c r="E16" s="0">
-        <x:v>72.0654</x:v>
+        <x:v>49.3474</x:v>
       </x:c>
       <x:c r="G16" s="0" t="s">
-        <x:v>36</x:v>
+        <x:v>47</x:v>
       </x:c>
       <x:c r="H16" s="0">
-        <x:v>0</x:v>
+        <x:v>24624.3526</x:v>
+      </x:c>
+      <x:c r="I16" s="0" t="s">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="J16" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="K16" s="0" t="s">
+        <x:v>21</x:v>
       </x:c>
       <x:c r="L16" s="0">
-        <x:v>0</x:v>
+        <x:v>499</x:v>
       </x:c>
     </x:row>
     <x:row r="17" spans="1:15">
       <x:c r="A17" s="0" t="s">
-        <x:v>42</x:v>
+        <x:v>56</x:v>
       </x:c>
       <x:c r="B17" s="0" t="s">
-        <x:v>16</x:v>
+        <x:v>57</x:v>
       </x:c>
       <x:c r="C17" s="0" t="s">
         <x:v>17</x:v>
       </x:c>
       <x:c r="D17" s="0">
-        <x:v>214</x:v>
+        <x:v>473</x:v>
       </x:c>
       <x:c r="E17" s="0">
-        <x:v>71.3859</x:v>
+        <x:v>11.1668</x:v>
       </x:c>
       <x:c r="G17" s="0" t="s">
-        <x:v>27</x:v>
+        <x:v>18</x:v>
       </x:c>
       <x:c r="H17" s="0">
-        <x:v>34693.5474</x:v>
+        <x:v>3227.2052</x:v>
       </x:c>
       <x:c r="I17" s="0" t="s">
         <x:v>19</x:v>
@@ -1190,71 +1379,80 @@
         <x:v>21</x:v>
       </x:c>
       <x:c r="L17" s="0">
-        <x:v>486</x:v>
+        <x:v>289</x:v>
       </x:c>
     </x:row>
     <x:row r="18" spans="1:15">
       <x:c r="A18" s="0" t="s">
-        <x:v>43</x:v>
+        <x:v>58</x:v>
       </x:c>
       <x:c r="B18" s="0" t="s">
-        <x:v>16</x:v>
+        <x:v>59</x:v>
       </x:c>
       <x:c r="C18" s="0" t="s">
         <x:v>17</x:v>
       </x:c>
+      <x:c r="D18" s="0">
+        <x:v>473</x:v>
+      </x:c>
       <x:c r="E18" s="0">
-        <x:v>41.7703</x:v>
+        <x:v>99.781</x:v>
       </x:c>
       <x:c r="G18" s="0" t="s">
-        <x:v>27</x:v>
+        <x:v>60</x:v>
       </x:c>
       <x:c r="H18" s="0">
-        <x:v>0</x:v>
+        <x:v>32428.825</x:v>
+      </x:c>
+      <x:c r="I18" s="0" t="s">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="J18" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="K18" s="0" t="s">
+        <x:v>21</x:v>
       </x:c>
       <x:c r="L18" s="0">
-        <x:v>0</x:v>
+        <x:v>325</x:v>
+      </x:c>
+      <x:c r="M18" s="0">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="N18" s="0" t="s">
+        <x:v>44</x:v>
+      </x:c>
+      <x:c r="O18" s="0" t="s">
+        <x:v>21</x:v>
       </x:c>
     </x:row>
     <x:row r="19" spans="1:15">
       <x:c r="A19" s="0" t="s">
+        <x:v>61</x:v>
+      </x:c>
+      <x:c r="B19" s="0" t="s">
+        <x:v>62</x:v>
+      </x:c>
+      <x:c r="C19" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="E19" s="0">
+        <x:v>91.3949</x:v>
+      </x:c>
+      <x:c r="G19" s="0" t="s">
+        <x:v>18</x:v>
+      </x:c>
+      <x:c r="H19" s="0">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="L19" s="0">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="M19" s="0">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="N19" s="0" t="s">
         <x:v>44</x:v>
-      </x:c>
-      <x:c r="B19" s="0" t="s">
-        <x:v>16</x:v>
-      </x:c>
-      <x:c r="C19" s="0" t="s">
-        <x:v>17</x:v>
-      </x:c>
-      <x:c r="D19" s="0">
-        <x:v>214</x:v>
-      </x:c>
-      <x:c r="E19" s="0">
-        <x:v>61.4794</x:v>
-      </x:c>
-      <x:c r="G19" s="0" t="s">
-        <x:v>32</x:v>
-      </x:c>
-      <x:c r="H19" s="0">
-        <x:v>23669.569</x:v>
-      </x:c>
-      <x:c r="I19" s="0" t="s">
-        <x:v>19</x:v>
-      </x:c>
-      <x:c r="J19" s="0" t="s">
-        <x:v>20</x:v>
-      </x:c>
-      <x:c r="K19" s="0" t="s">
-        <x:v>21</x:v>
-      </x:c>
-      <x:c r="L19" s="0">
-        <x:v>385</x:v>
-      </x:c>
-      <x:c r="M19" s="0">
-        <x:v>4</x:v>
-      </x:c>
-      <x:c r="N19" s="0" t="s">
-        <x:v>22</x:v>
       </x:c>
       <x:c r="O19" s="0" t="s">
         <x:v>21</x:v>
@@ -1262,25 +1460,25 @@
     </x:row>
     <x:row r="20" spans="1:15">
       <x:c r="A20" s="0" t="s">
-        <x:v>45</x:v>
+        <x:v>63</x:v>
       </x:c>
       <x:c r="B20" s="0" t="s">
-        <x:v>16</x:v>
+        <x:v>64</x:v>
       </x:c>
       <x:c r="C20" s="0" t="s">
         <x:v>17</x:v>
       </x:c>
       <x:c r="D20" s="0">
-        <x:v>214</x:v>
+        <x:v>473</x:v>
       </x:c>
       <x:c r="E20" s="0">
-        <x:v>53.1757</x:v>
+        <x:v>34.3438</x:v>
       </x:c>
       <x:c r="G20" s="0" t="s">
-        <x:v>46</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="H20" s="0">
-        <x:v>6381.084</x:v>
+        <x:v>15969.867</x:v>
       </x:c>
       <x:c r="I20" s="0" t="s">
         <x:v>19</x:v>
@@ -1292,94 +1490,79 @@
         <x:v>21</x:v>
       </x:c>
       <x:c r="L20" s="0">
-        <x:v>120</x:v>
+        <x:v>465</x:v>
       </x:c>
     </x:row>
     <x:row r="21" spans="1:15">
       <x:c r="A21" s="0" t="s">
-        <x:v>47</x:v>
+        <x:v>65</x:v>
       </x:c>
       <x:c r="B21" s="0" t="s">
-        <x:v>16</x:v>
+        <x:v>66</x:v>
       </x:c>
       <x:c r="C21" s="0" t="s">
         <x:v>17</x:v>
       </x:c>
-      <x:c r="D21" s="0">
-        <x:v>214</x:v>
-      </x:c>
       <x:c r="E21" s="0">
-        <x:v>77.3767</x:v>
+        <x:v>87.1003</x:v>
       </x:c>
       <x:c r="G21" s="0" t="s">
-        <x:v>27</x:v>
+        <x:v>18</x:v>
       </x:c>
       <x:c r="H21" s="0">
-        <x:v>29790.0295</x:v>
-      </x:c>
-      <x:c r="I21" s="0" t="s">
-        <x:v>19</x:v>
-      </x:c>
-      <x:c r="J21" s="0" t="s">
-        <x:v>20</x:v>
-      </x:c>
-      <x:c r="K21" s="0" t="s">
-        <x:v>21</x:v>
+        <x:v>0</x:v>
       </x:c>
       <x:c r="L21" s="0">
-        <x:v>385</x:v>
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="M21" s="0">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="N21" s="0" t="s">
+        <x:v>44</x:v>
+      </x:c>
+      <x:c r="O21" s="0" t="s">
+        <x:v>21</x:v>
       </x:c>
     </x:row>
     <x:row r="22" spans="1:15">
       <x:c r="A22" s="0" t="s">
-        <x:v>48</x:v>
+        <x:v>67</x:v>
       </x:c>
       <x:c r="B22" s="0" t="s">
-        <x:v>16</x:v>
+        <x:v>68</x:v>
       </x:c>
       <x:c r="C22" s="0" t="s">
         <x:v>17</x:v>
       </x:c>
-      <x:c r="D22" s="0">
-        <x:v>214</x:v>
-      </x:c>
       <x:c r="E22" s="0">
-        <x:v>70.3522</x:v>
+        <x:v>88.0201</x:v>
       </x:c>
       <x:c r="G22" s="0" t="s">
-        <x:v>46</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="H22" s="0">
-        <x:v>25608.2008</x:v>
-      </x:c>
-      <x:c r="I22" s="0" t="s">
-        <x:v>19</x:v>
-      </x:c>
-      <x:c r="J22" s="0" t="s">
-        <x:v>20</x:v>
-      </x:c>
-      <x:c r="K22" s="0" t="s">
-        <x:v>21</x:v>
+        <x:v>0</x:v>
       </x:c>
       <x:c r="L22" s="0">
-        <x:v>364</x:v>
+        <x:v>0</x:v>
       </x:c>
     </x:row>
     <x:row r="23" spans="1:15">
       <x:c r="A23" s="0" t="s">
-        <x:v>49</x:v>
+        <x:v>69</x:v>
       </x:c>
       <x:c r="B23" s="0" t="s">
-        <x:v>16</x:v>
+        <x:v>70</x:v>
       </x:c>
       <x:c r="C23" s="0" t="s">
         <x:v>17</x:v>
       </x:c>
       <x:c r="E23" s="0">
-        <x:v>17.1328</x:v>
+        <x:v>45.1307</x:v>
       </x:c>
       <x:c r="G23" s="0" t="s">
-        <x:v>18</x:v>
+        <x:v>32</x:v>
       </x:c>
       <x:c r="H23" s="0">
         <x:v>0</x:v>
@@ -1390,48 +1573,57 @@
     </x:row>
     <x:row r="24" spans="1:15">
       <x:c r="A24" s="0" t="s">
-        <x:v>50</x:v>
+        <x:v>71</x:v>
       </x:c>
       <x:c r="B24" s="0" t="s">
-        <x:v>16</x:v>
+        <x:v>72</x:v>
       </x:c>
       <x:c r="C24" s="0" t="s">
         <x:v>17</x:v>
       </x:c>
       <x:c r="E24" s="0">
-        <x:v>39.766</x:v>
+        <x:v>96.5419</x:v>
       </x:c>
       <x:c r="G24" s="0" t="s">
-        <x:v>46</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="H24" s="0">
         <x:v>0</x:v>
       </x:c>
       <x:c r="L24" s="0">
         <x:v>0</x:v>
+      </x:c>
+      <x:c r="M24" s="0">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="N24" s="0" t="s">
+        <x:v>44</x:v>
+      </x:c>
+      <x:c r="O24" s="0" t="s">
+        <x:v>21</x:v>
       </x:c>
     </x:row>
     <x:row r="25" spans="1:15">
       <x:c r="A25" s="0" t="s">
-        <x:v>51</x:v>
+        <x:v>73</x:v>
       </x:c>
       <x:c r="B25" s="0" t="s">
-        <x:v>16</x:v>
+        <x:v>74</x:v>
       </x:c>
       <x:c r="C25" s="0" t="s">
         <x:v>17</x:v>
       </x:c>
       <x:c r="D25" s="0">
-        <x:v>214</x:v>
+        <x:v>473</x:v>
       </x:c>
       <x:c r="E25" s="0">
-        <x:v>47.7875</x:v>
+        <x:v>96.4492</x:v>
       </x:c>
       <x:c r="G25" s="0" t="s">
-        <x:v>18</x:v>
+        <x:v>47</x:v>
       </x:c>
       <x:c r="H25" s="0">
-        <x:v>6785.825</x:v>
+        <x:v>12345.4976</x:v>
       </x:c>
       <x:c r="I25" s="0" t="s">
         <x:v>19</x:v>
@@ -1443,13 +1635,13 @@
         <x:v>21</x:v>
       </x:c>
       <x:c r="L25" s="0">
-        <x:v>142</x:v>
+        <x:v>128</x:v>
       </x:c>
       <x:c r="M25" s="0">
-        <x:v>7</x:v>
+        <x:v>5</x:v>
       </x:c>
       <x:c r="N25" s="0" t="s">
-        <x:v>22</x:v>
+        <x:v>44</x:v>
       </x:c>
       <x:c r="O25" s="0" t="s">
         <x:v>21</x:v>
@@ -1457,25 +1649,25 @@
     </x:row>
     <x:row r="26" spans="1:15">
       <x:c r="A26" s="0" t="s">
-        <x:v>52</x:v>
+        <x:v>75</x:v>
       </x:c>
       <x:c r="B26" s="0" t="s">
-        <x:v>16</x:v>
+        <x:v>76</x:v>
       </x:c>
       <x:c r="C26" s="0" t="s">
         <x:v>17</x:v>
       </x:c>
       <x:c r="D26" s="0">
-        <x:v>214</x:v>
+        <x:v>473</x:v>
       </x:c>
       <x:c r="E26" s="0">
-        <x:v>86.7105</x:v>
+        <x:v>17.4921</x:v>
       </x:c>
       <x:c r="G26" s="0" t="s">
-        <x:v>32</x:v>
+        <x:v>18</x:v>
       </x:c>
       <x:c r="H26" s="0">
-        <x:v>29481.57</x:v>
+        <x:v>87.4605</x:v>
       </x:c>
       <x:c r="I26" s="0" t="s">
         <x:v>19</x:v>
@@ -1487,83 +1679,53 @@
         <x:v>21</x:v>
       </x:c>
       <x:c r="L26" s="0">
-        <x:v>340</x:v>
-      </x:c>
-      <x:c r="M26" s="0">
-        <x:v>7</x:v>
-      </x:c>
-      <x:c r="N26" s="0" t="s">
-        <x:v>22</x:v>
-      </x:c>
-      <x:c r="O26" s="0" t="s">
-        <x:v>21</x:v>
+        <x:v>5</x:v>
       </x:c>
     </x:row>
     <x:row r="27" spans="1:15">
       <x:c r="A27" s="0" t="s">
-        <x:v>53</x:v>
+        <x:v>77</x:v>
       </x:c>
       <x:c r="B27" s="0" t="s">
-        <x:v>16</x:v>
+        <x:v>78</x:v>
       </x:c>
       <x:c r="C27" s="0" t="s">
         <x:v>17</x:v>
       </x:c>
-      <x:c r="D27" s="0">
-        <x:v>214</x:v>
-      </x:c>
       <x:c r="E27" s="0">
-        <x:v>1.1349</x:v>
+        <x:v>83.2273</x:v>
       </x:c>
       <x:c r="G27" s="0" t="s">
-        <x:v>27</x:v>
+        <x:v>32</x:v>
       </x:c>
       <x:c r="H27" s="0">
-        <x:v>363.168</x:v>
-      </x:c>
-      <x:c r="I27" s="0" t="s">
-        <x:v>19</x:v>
-      </x:c>
-      <x:c r="J27" s="0" t="s">
-        <x:v>20</x:v>
-      </x:c>
-      <x:c r="K27" s="0" t="s">
-        <x:v>21</x:v>
+        <x:v>0</x:v>
       </x:c>
       <x:c r="L27" s="0">
-        <x:v>320</x:v>
-      </x:c>
-      <x:c r="M27" s="0">
-        <x:v>1</x:v>
-      </x:c>
-      <x:c r="N27" s="0" t="s">
-        <x:v>22</x:v>
-      </x:c>
-      <x:c r="O27" s="0" t="s">
-        <x:v>21</x:v>
+        <x:v>0</x:v>
       </x:c>
     </x:row>
     <x:row r="28" spans="1:15">
       <x:c r="A28" s="0" t="s">
-        <x:v>54</x:v>
+        <x:v>79</x:v>
       </x:c>
       <x:c r="B28" s="0" t="s">
-        <x:v>16</x:v>
+        <x:v>80</x:v>
       </x:c>
       <x:c r="C28" s="0" t="s">
         <x:v>17</x:v>
       </x:c>
       <x:c r="D28" s="0">
-        <x:v>214</x:v>
+        <x:v>473</x:v>
       </x:c>
       <x:c r="E28" s="0">
-        <x:v>56.9567</x:v>
+        <x:v>67.1772</x:v>
       </x:c>
       <x:c r="G28" s="0" t="s">
-        <x:v>24</x:v>
+        <x:v>60</x:v>
       </x:c>
       <x:c r="H28" s="0">
-        <x:v>17371.7935</x:v>
+        <x:v>2351.202</x:v>
       </x:c>
       <x:c r="I28" s="0" t="s">
         <x:v>19</x:v>
@@ -1575,57 +1737,48 @@
         <x:v>21</x:v>
       </x:c>
       <x:c r="L28" s="0">
-        <x:v>305</x:v>
-      </x:c>
-      <x:c r="M28" s="0">
-        <x:v>1</x:v>
-      </x:c>
-      <x:c r="N28" s="0" t="s">
-        <x:v>22</x:v>
-      </x:c>
-      <x:c r="O28" s="0" t="s">
-        <x:v>21</x:v>
+        <x:v>35</x:v>
       </x:c>
     </x:row>
     <x:row r="29" spans="1:15">
       <x:c r="A29" s="0" t="s">
-        <x:v>55</x:v>
+        <x:v>81</x:v>
       </x:c>
       <x:c r="B29" s="0" t="s">
-        <x:v>16</x:v>
+        <x:v>82</x:v>
       </x:c>
       <x:c r="C29" s="0" t="s">
         <x:v>17</x:v>
       </x:c>
       <x:c r="D29" s="0">
-        <x:v>214</x:v>
+        <x:v>473</x:v>
       </x:c>
       <x:c r="E29" s="0">
-        <x:v>17.3087</x:v>
+        <x:v>45.3543</x:v>
       </x:c>
       <x:c r="G29" s="0" t="s">
-        <x:v>36</x:v>
+        <x:v>18</x:v>
       </x:c>
       <x:c r="H29" s="0">
-        <x:v>432.7175</x:v>
+        <x:v>13833.0615</x:v>
       </x:c>
       <x:c r="I29" s="0" t="s">
-        <x:v>56</x:v>
+        <x:v>19</x:v>
       </x:c>
       <x:c r="J29" s="0" t="s">
-        <x:v>57</x:v>
+        <x:v>20</x:v>
       </x:c>
       <x:c r="K29" s="0" t="s">
         <x:v>21</x:v>
       </x:c>
       <x:c r="L29" s="0">
-        <x:v>25</x:v>
+        <x:v>305</x:v>
       </x:c>
       <x:c r="M29" s="0">
-        <x:v>1</x:v>
+        <x:v>4</x:v>
       </x:c>
       <x:c r="N29" s="0" t="s">
-        <x:v>22</x:v>
+        <x:v>44</x:v>
       </x:c>
       <x:c r="O29" s="0" t="s">
         <x:v>21</x:v>
@@ -1633,98 +1786,74 @@
     </x:row>
     <x:row r="30" spans="1:15">
       <x:c r="A30" s="0" t="s">
-        <x:v>58</x:v>
+        <x:v>83</x:v>
       </x:c>
       <x:c r="B30" s="0" t="s">
-        <x:v>16</x:v>
+        <x:v>84</x:v>
       </x:c>
       <x:c r="C30" s="0" t="s">
         <x:v>17</x:v>
       </x:c>
-      <x:c r="D30" s="0">
-        <x:v>214</x:v>
-      </x:c>
       <x:c r="E30" s="0">
-        <x:v>90.9597</x:v>
+        <x:v>49.3463</x:v>
       </x:c>
       <x:c r="G30" s="0" t="s">
-        <x:v>32</x:v>
+        <x:v>18</x:v>
       </x:c>
       <x:c r="H30" s="0">
-        <x:v>16645.6251</x:v>
-      </x:c>
-      <x:c r="I30" s="0" t="s">
-        <x:v>19</x:v>
-      </x:c>
-      <x:c r="J30" s="0" t="s">
-        <x:v>20</x:v>
-      </x:c>
-      <x:c r="K30" s="0" t="s">
-        <x:v>21</x:v>
+        <x:v>0</x:v>
       </x:c>
       <x:c r="L30" s="0">
-        <x:v>183</x:v>
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="M30" s="0">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="N30" s="0" t="s">
+        <x:v>44</x:v>
+      </x:c>
+      <x:c r="O30" s="0" t="s">
+        <x:v>21</x:v>
       </x:c>
     </x:row>
     <x:row r="31" spans="1:15">
       <x:c r="A31" s="0" t="s">
-        <x:v>59</x:v>
+        <x:v>85</x:v>
       </x:c>
       <x:c r="B31" s="0" t="s">
-        <x:v>16</x:v>
+        <x:v>86</x:v>
       </x:c>
       <x:c r="C31" s="0" t="s">
         <x:v>17</x:v>
       </x:c>
-      <x:c r="D31" s="0">
-        <x:v>214</x:v>
-      </x:c>
       <x:c r="E31" s="0">
-        <x:v>81.2159</x:v>
+        <x:v>46.3934</x:v>
       </x:c>
       <x:c r="G31" s="0" t="s">
-        <x:v>46</x:v>
+        <x:v>27</x:v>
       </x:c>
       <x:c r="H31" s="0">
-        <x:v>9745.908</x:v>
-      </x:c>
-      <x:c r="I31" s="0" t="s">
-        <x:v>19</x:v>
-      </x:c>
-      <x:c r="J31" s="0" t="s">
-        <x:v>20</x:v>
-      </x:c>
-      <x:c r="K31" s="0" t="s">
-        <x:v>21</x:v>
+        <x:v>0</x:v>
       </x:c>
       <x:c r="L31" s="0">
-        <x:v>120</x:v>
-      </x:c>
-      <x:c r="M31" s="0">
-        <x:v>4</x:v>
-      </x:c>
-      <x:c r="N31" s="0" t="s">
-        <x:v>22</x:v>
-      </x:c>
-      <x:c r="O31" s="0" t="s">
-        <x:v>21</x:v>
+        <x:v>0</x:v>
       </x:c>
     </x:row>
     <x:row r="32" spans="1:15">
       <x:c r="A32" s="0" t="s">
-        <x:v>60</x:v>
+        <x:v>87</x:v>
       </x:c>
       <x:c r="B32" s="0" t="s">
-        <x:v>16</x:v>
+        <x:v>88</x:v>
       </x:c>
       <x:c r="C32" s="0" t="s">
         <x:v>17</x:v>
       </x:c>
       <x:c r="E32" s="0">
-        <x:v>67.6266</x:v>
+        <x:v>18.3081</x:v>
       </x:c>
       <x:c r="G32" s="0" t="s">
-        <x:v>46</x:v>
+        <x:v>27</x:v>
       </x:c>
       <x:c r="H32" s="0">
         <x:v>0</x:v>
@@ -1735,25 +1864,25 @@
     </x:row>
     <x:row r="33" spans="1:15">
       <x:c r="A33" s="0" t="s">
-        <x:v>61</x:v>
+        <x:v>89</x:v>
       </x:c>
       <x:c r="B33" s="0" t="s">
-        <x:v>16</x:v>
+        <x:v>90</x:v>
       </x:c>
       <x:c r="C33" s="0" t="s">
         <x:v>17</x:v>
       </x:c>
       <x:c r="D33" s="0">
-        <x:v>214</x:v>
+        <x:v>473</x:v>
       </x:c>
       <x:c r="E33" s="0">
-        <x:v>42.8331</x:v>
+        <x:v>78.0741</x:v>
       </x:c>
       <x:c r="G33" s="0" t="s">
-        <x:v>36</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="H33" s="0">
-        <x:v>17390.2386</x:v>
+        <x:v>9993.4848</x:v>
       </x:c>
       <x:c r="I33" s="0" t="s">
         <x:v>19</x:v>
@@ -1765,53 +1894,83 @@
         <x:v>21</x:v>
       </x:c>
       <x:c r="L33" s="0">
-        <x:v>406</x:v>
+        <x:v>128</x:v>
+      </x:c>
+      <x:c r="M33" s="0">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="N33" s="0" t="s">
+        <x:v>44</x:v>
+      </x:c>
+      <x:c r="O33" s="0" t="s">
+        <x:v>21</x:v>
       </x:c>
     </x:row>
     <x:row r="34" spans="1:15">
       <x:c r="A34" s="0" t="s">
-        <x:v>62</x:v>
+        <x:v>91</x:v>
       </x:c>
       <x:c r="B34" s="0" t="s">
-        <x:v>16</x:v>
+        <x:v>92</x:v>
       </x:c>
       <x:c r="C34" s="0" t="s">
         <x:v>17</x:v>
       </x:c>
+      <x:c r="D34" s="0">
+        <x:v>473</x:v>
+      </x:c>
       <x:c r="E34" s="0">
-        <x:v>82.1277</x:v>
+        <x:v>9.4865</x:v>
       </x:c>
       <x:c r="G34" s="0" t="s">
-        <x:v>18</x:v>
+        <x:v>27</x:v>
       </x:c>
       <x:c r="H34" s="0">
-        <x:v>0</x:v>
+        <x:v>2637.247</x:v>
+      </x:c>
+      <x:c r="I34" s="0" t="s">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="J34" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="K34" s="0" t="s">
+        <x:v>21</x:v>
       </x:c>
       <x:c r="L34" s="0">
-        <x:v>0</x:v>
+        <x:v>278</x:v>
+      </x:c>
+      <x:c r="M34" s="0">
+        <x:v>2</x:v>
+      </x:c>
+      <x:c r="N34" s="0" t="s">
+        <x:v>44</x:v>
+      </x:c>
+      <x:c r="O34" s="0" t="s">
+        <x:v>21</x:v>
       </x:c>
     </x:row>
     <x:row r="35" spans="1:15">
       <x:c r="A35" s="0" t="s">
-        <x:v>63</x:v>
+        <x:v>93</x:v>
       </x:c>
       <x:c r="B35" s="0" t="s">
-        <x:v>16</x:v>
+        <x:v>94</x:v>
       </x:c>
       <x:c r="C35" s="0" t="s">
         <x:v>17</x:v>
       </x:c>
       <x:c r="D35" s="0">
-        <x:v>214</x:v>
+        <x:v>473</x:v>
       </x:c>
       <x:c r="E35" s="0">
-        <x:v>11.7536</x:v>
+        <x:v>97.1158</x:v>
       </x:c>
       <x:c r="G35" s="0" t="s">
-        <x:v>32</x:v>
+        <x:v>18</x:v>
       </x:c>
       <x:c r="H35" s="0">
-        <x:v>1410.432</x:v>
+        <x:v>32436.6772</x:v>
       </x:c>
       <x:c r="I35" s="0" t="s">
         <x:v>19</x:v>
@@ -1823,30 +1982,39 @@
         <x:v>21</x:v>
       </x:c>
       <x:c r="L35" s="0">
-        <x:v>120</x:v>
+        <x:v>334</x:v>
+      </x:c>
+      <x:c r="M35" s="0">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="N35" s="0" t="s">
+        <x:v>44</x:v>
+      </x:c>
+      <x:c r="O35" s="0" t="s">
+        <x:v>21</x:v>
       </x:c>
     </x:row>
     <x:row r="36" spans="1:15">
       <x:c r="A36" s="0" t="s">
-        <x:v>64</x:v>
+        <x:v>95</x:v>
       </x:c>
       <x:c r="B36" s="0" t="s">
-        <x:v>16</x:v>
+        <x:v>96</x:v>
       </x:c>
       <x:c r="C36" s="0" t="s">
         <x:v>17</x:v>
       </x:c>
       <x:c r="D36" s="0">
-        <x:v>214</x:v>
+        <x:v>473</x:v>
       </x:c>
       <x:c r="E36" s="0">
-        <x:v>80.0882</x:v>
+        <x:v>68.4187</x:v>
       </x:c>
       <x:c r="G36" s="0" t="s">
-        <x:v>46</x:v>
+        <x:v>47</x:v>
       </x:c>
       <x:c r="H36" s="0">
-        <x:v>11132.2598</x:v>
+        <x:v>33251.4882</x:v>
       </x:c>
       <x:c r="I36" s="0" t="s">
         <x:v>19</x:v>
@@ -1858,68 +2026,47 @@
         <x:v>21</x:v>
       </x:c>
       <x:c r="L36" s="0">
-        <x:v>139</x:v>
-      </x:c>
-      <x:c r="M36" s="0">
-        <x:v>1</x:v>
-      </x:c>
-      <x:c r="N36" s="0" t="s">
-        <x:v>22</x:v>
-      </x:c>
-      <x:c r="O36" s="0" t="s">
-        <x:v>21</x:v>
+        <x:v>486</x:v>
       </x:c>
     </x:row>
     <x:row r="37" spans="1:15">
       <x:c r="A37" s="0" t="s">
-        <x:v>65</x:v>
+        <x:v>97</x:v>
       </x:c>
       <x:c r="B37" s="0" t="s">
-        <x:v>16</x:v>
+        <x:v>98</x:v>
       </x:c>
       <x:c r="C37" s="0" t="s">
         <x:v>17</x:v>
       </x:c>
-      <x:c r="D37" s="0">
-        <x:v>214</x:v>
-      </x:c>
       <x:c r="E37" s="0">
-        <x:v>8.2778</x:v>
+        <x:v>12.9254</x:v>
       </x:c>
       <x:c r="G37" s="0" t="s">
-        <x:v>18</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="H37" s="0">
-        <x:v>902.2802</x:v>
-      </x:c>
-      <x:c r="I37" s="0" t="s">
-        <x:v>19</x:v>
-      </x:c>
-      <x:c r="J37" s="0" t="s">
-        <x:v>20</x:v>
-      </x:c>
-      <x:c r="K37" s="0" t="s">
-        <x:v>21</x:v>
+        <x:v>0</x:v>
       </x:c>
       <x:c r="L37" s="0">
-        <x:v>109</x:v>
+        <x:v>0</x:v>
       </x:c>
     </x:row>
     <x:row r="38" spans="1:15">
       <x:c r="A38" s="0" t="s">
-        <x:v>66</x:v>
+        <x:v>99</x:v>
       </x:c>
       <x:c r="B38" s="0" t="s">
-        <x:v>16</x:v>
+        <x:v>100</x:v>
       </x:c>
       <x:c r="C38" s="0" t="s">
         <x:v>17</x:v>
       </x:c>
       <x:c r="E38" s="0">
-        <x:v>11.8474</x:v>
+        <x:v>94.3892</x:v>
       </x:c>
       <x:c r="G38" s="0" t="s">
-        <x:v>36</x:v>
+        <x:v>32</x:v>
       </x:c>
       <x:c r="H38" s="0">
         <x:v>0</x:v>
@@ -1928,10 +2075,10 @@
         <x:v>0</x:v>
       </x:c>
       <x:c r="M38" s="0">
-        <x:v>7</x:v>
+        <x:v>4</x:v>
       </x:c>
       <x:c r="N38" s="0" t="s">
-        <x:v>22</x:v>
+        <x:v>44</x:v>
       </x:c>
       <x:c r="O38" s="0" t="s">
         <x:v>21</x:v>
@@ -1939,60 +2086,57 @@
     </x:row>
     <x:row r="39" spans="1:15">
       <x:c r="A39" s="0" t="s">
-        <x:v>67</x:v>
+        <x:v>101</x:v>
       </x:c>
       <x:c r="B39" s="0" t="s">
-        <x:v>16</x:v>
+        <x:v>102</x:v>
       </x:c>
       <x:c r="C39" s="0" t="s">
         <x:v>17</x:v>
       </x:c>
-      <x:c r="D39" s="0">
-        <x:v>214</x:v>
-      </x:c>
       <x:c r="E39" s="0">
-        <x:v>36.8709</x:v>
+        <x:v>91.1785</x:v>
       </x:c>
       <x:c r="G39" s="0" t="s">
-        <x:v>27</x:v>
+        <x:v>32</x:v>
       </x:c>
       <x:c r="H39" s="0">
-        <x:v>9180.8541</x:v>
-      </x:c>
-      <x:c r="I39" s="0" t="s">
-        <x:v>19</x:v>
-      </x:c>
-      <x:c r="J39" s="0" t="s">
-        <x:v>20</x:v>
-      </x:c>
-      <x:c r="K39" s="0" t="s">
-        <x:v>21</x:v>
+        <x:v>0</x:v>
       </x:c>
       <x:c r="L39" s="0">
-        <x:v>249</x:v>
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="M39" s="0">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="N39" s="0" t="s">
+        <x:v>44</x:v>
+      </x:c>
+      <x:c r="O39" s="0" t="s">
+        <x:v>21</x:v>
       </x:c>
     </x:row>
     <x:row r="40" spans="1:15">
       <x:c r="A40" s="0" t="s">
-        <x:v>68</x:v>
+        <x:v>103</x:v>
       </x:c>
       <x:c r="B40" s="0" t="s">
-        <x:v>16</x:v>
+        <x:v>104</x:v>
       </x:c>
       <x:c r="C40" s="0" t="s">
         <x:v>17</x:v>
       </x:c>
       <x:c r="D40" s="0">
-        <x:v>214</x:v>
+        <x:v>473</x:v>
       </x:c>
       <x:c r="E40" s="0">
-        <x:v>28.2839</x:v>
+        <x:v>74.1369</x:v>
       </x:c>
       <x:c r="G40" s="0" t="s">
-        <x:v>36</x:v>
+        <x:v>18</x:v>
       </x:c>
       <x:c r="H40" s="0">
-        <x:v>4016.3138</x:v>
+        <x:v>2594.7915</x:v>
       </x:c>
       <x:c r="I40" s="0" t="s">
         <x:v>19</x:v>
@@ -2004,62 +2148,74 @@
         <x:v>21</x:v>
       </x:c>
       <x:c r="L40" s="0">
-        <x:v>142</x:v>
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="M40" s="0">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="N40" s="0" t="s">
+        <x:v>44</x:v>
+      </x:c>
+      <x:c r="O40" s="0" t="s">
+        <x:v>21</x:v>
       </x:c>
     </x:row>
     <x:row r="41" spans="1:15">
       <x:c r="A41" s="0" t="s">
-        <x:v>69</x:v>
+        <x:v>105</x:v>
       </x:c>
       <x:c r="B41" s="0" t="s">
-        <x:v>16</x:v>
+        <x:v>106</x:v>
       </x:c>
       <x:c r="C41" s="0" t="s">
         <x:v>17</x:v>
       </x:c>
+      <x:c r="D41" s="0">
+        <x:v>473</x:v>
+      </x:c>
       <x:c r="E41" s="0">
-        <x:v>47.2759</x:v>
+        <x:v>30.2469</x:v>
       </x:c>
       <x:c r="G41" s="0" t="s">
-        <x:v>30</x:v>
+        <x:v>60</x:v>
       </x:c>
       <x:c r="H41" s="0">
-        <x:v>0</x:v>
+        <x:v>7531.4781</x:v>
+      </x:c>
+      <x:c r="I41" s="0" t="s">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="J41" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="K41" s="0" t="s">
+        <x:v>21</x:v>
       </x:c>
       <x:c r="L41" s="0">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="M41" s="0">
-        <x:v>5</x:v>
-      </x:c>
-      <x:c r="N41" s="0" t="s">
-        <x:v>22</x:v>
-      </x:c>
-      <x:c r="O41" s="0" t="s">
-        <x:v>21</x:v>
+        <x:v>249</x:v>
       </x:c>
     </x:row>
     <x:row r="42" spans="1:15">
       <x:c r="A42" s="0" t="s">
-        <x:v>70</x:v>
+        <x:v>107</x:v>
       </x:c>
       <x:c r="B42" s="0" t="s">
-        <x:v>16</x:v>
+        <x:v>108</x:v>
       </x:c>
       <x:c r="C42" s="0" t="s">
         <x:v>17</x:v>
       </x:c>
       <x:c r="D42" s="0">
-        <x:v>214</x:v>
+        <x:v>473</x:v>
       </x:c>
       <x:c r="E42" s="0">
-        <x:v>35.0529</x:v>
+        <x:v>8.481</x:v>
       </x:c>
       <x:c r="G42" s="0" t="s">
-        <x:v>46</x:v>
+        <x:v>60</x:v>
       </x:c>
       <x:c r="H42" s="0">
-        <x:v>12619.044</x:v>
+        <x:v>4206.576</x:v>
       </x:c>
       <x:c r="I42" s="0" t="s">
         <x:v>19</x:v>
@@ -2071,30 +2227,39 @@
         <x:v>21</x:v>
       </x:c>
       <x:c r="L42" s="0">
-        <x:v>360</x:v>
+        <x:v>496</x:v>
+      </x:c>
+      <x:c r="M42" s="0">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="N42" s="0" t="s">
+        <x:v>44</x:v>
+      </x:c>
+      <x:c r="O42" s="0" t="s">
+        <x:v>21</x:v>
       </x:c>
     </x:row>
     <x:row r="43" spans="1:15">
       <x:c r="A43" s="0" t="s">
-        <x:v>71</x:v>
+        <x:v>109</x:v>
       </x:c>
       <x:c r="B43" s="0" t="s">
-        <x:v>16</x:v>
+        <x:v>110</x:v>
       </x:c>
       <x:c r="C43" s="0" t="s">
         <x:v>17</x:v>
       </x:c>
       <x:c r="D43" s="0">
-        <x:v>214</x:v>
+        <x:v>473</x:v>
       </x:c>
       <x:c r="E43" s="0">
-        <x:v>35.5605</x:v>
+        <x:v>89.4185</x:v>
       </x:c>
       <x:c r="G43" s="0" t="s">
-        <x:v>36</x:v>
+        <x:v>18</x:v>
       </x:c>
       <x:c r="H43" s="0">
-        <x:v>17282.403</x:v>
+        <x:v>29865.779</x:v>
       </x:c>
       <x:c r="I43" s="0" t="s">
         <x:v>19</x:v>
@@ -2106,53 +2271,74 @@
         <x:v>21</x:v>
       </x:c>
       <x:c r="L43" s="0">
-        <x:v>486</x:v>
+        <x:v>334</x:v>
       </x:c>
     </x:row>
     <x:row r="44" spans="1:15">
       <x:c r="A44" s="0" t="s">
-        <x:v>72</x:v>
+        <x:v>111</x:v>
       </x:c>
       <x:c r="B44" s="0" t="s">
-        <x:v>16</x:v>
+        <x:v>112</x:v>
       </x:c>
       <x:c r="C44" s="0" t="s">
         <x:v>17</x:v>
       </x:c>
+      <x:c r="D44" s="0">
+        <x:v>473</x:v>
+      </x:c>
       <x:c r="E44" s="0">
-        <x:v>47.8815</x:v>
+        <x:v>67.9979</x:v>
       </x:c>
       <x:c r="G44" s="0" t="s">
-        <x:v>36</x:v>
+        <x:v>27</x:v>
       </x:c>
       <x:c r="H44" s="0">
-        <x:v>0</x:v>
+        <x:v>23867.2629</x:v>
+      </x:c>
+      <x:c r="I44" s="0" t="s">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="J44" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="K44" s="0" t="s">
+        <x:v>21</x:v>
       </x:c>
       <x:c r="L44" s="0">
-        <x:v>0</x:v>
+        <x:v>351</x:v>
+      </x:c>
+      <x:c r="M44" s="0">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="N44" s="0" t="s">
+        <x:v>44</x:v>
+      </x:c>
+      <x:c r="O44" s="0" t="s">
+        <x:v>21</x:v>
       </x:c>
     </x:row>
     <x:row r="45" spans="1:15">
       <x:c r="A45" s="0" t="s">
-        <x:v>73</x:v>
+        <x:v>113</x:v>
       </x:c>
       <x:c r="B45" s="0" t="s">
-        <x:v>16</x:v>
+        <x:v>114</x:v>
       </x:c>
       <x:c r="C45" s="0" t="s">
         <x:v>17</x:v>
       </x:c>
       <x:c r="D45" s="0">
-        <x:v>214</x:v>
+        <x:v>473</x:v>
       </x:c>
       <x:c r="E45" s="0">
-        <x:v>93.5851</x:v>
+        <x:v>97.3209</x:v>
       </x:c>
       <x:c r="G45" s="0" t="s">
-        <x:v>32</x:v>
+        <x:v>27</x:v>
       </x:c>
       <x:c r="H45" s="0">
-        <x:v>36030.2635</x:v>
+        <x:v>27055.2102</x:v>
       </x:c>
       <x:c r="I45" s="0" t="s">
         <x:v>19</x:v>
@@ -2164,120 +2350,132 @@
         <x:v>21</x:v>
       </x:c>
       <x:c r="L45" s="0">
-        <x:v>385</x:v>
-      </x:c>
-      <x:c r="M45" s="0">
-        <x:v>1</x:v>
-      </x:c>
-      <x:c r="N45" s="0" t="s">
-        <x:v>22</x:v>
-      </x:c>
-      <x:c r="O45" s="0" t="s">
-        <x:v>21</x:v>
+        <x:v>278</x:v>
       </x:c>
     </x:row>
     <x:row r="46" spans="1:15">
       <x:c r="A46" s="0" t="s">
-        <x:v>74</x:v>
+        <x:v>115</x:v>
       </x:c>
       <x:c r="B46" s="0" t="s">
-        <x:v>16</x:v>
+        <x:v>116</x:v>
       </x:c>
       <x:c r="C46" s="0" t="s">
         <x:v>17</x:v>
       </x:c>
+      <x:c r="D46" s="0">
+        <x:v>473</x:v>
+      </x:c>
       <x:c r="E46" s="0">
-        <x:v>1.3955</x:v>
+        <x:v>81.6868</x:v>
       </x:c>
       <x:c r="G46" s="0" t="s">
-        <x:v>18</x:v>
+        <x:v>60</x:v>
       </x:c>
       <x:c r="H46" s="0">
-        <x:v>0</x:v>
+        <x:v>816.868</x:v>
+      </x:c>
+      <x:c r="I46" s="0" t="s">
+        <x:v>117</x:v>
+      </x:c>
+      <x:c r="J46" s="0" t="s">
+        <x:v>118</x:v>
+      </x:c>
+      <x:c r="K46" s="0" t="s">
+        <x:v>21</x:v>
       </x:c>
       <x:c r="L46" s="0">
-        <x:v>0</x:v>
+        <x:v>10</x:v>
       </x:c>
     </x:row>
     <x:row r="47" spans="1:15">
       <x:c r="A47" s="0" t="s">
-        <x:v>75</x:v>
+        <x:v>119</x:v>
       </x:c>
       <x:c r="B47" s="0" t="s">
-        <x:v>16</x:v>
+        <x:v>120</x:v>
       </x:c>
       <x:c r="C47" s="0" t="s">
         <x:v>17</x:v>
       </x:c>
       <x:c r="D47" s="0">
-        <x:v>214</x:v>
+        <x:v>473</x:v>
       </x:c>
       <x:c r="E47" s="0">
-        <x:v>11.8063</x:v>
+        <x:v>23.2202</x:v>
       </x:c>
       <x:c r="G47" s="0" t="s">
-        <x:v>32</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="H47" s="0">
-        <x:v>118.063</x:v>
+        <x:v>8637.9144</x:v>
       </x:c>
       <x:c r="I47" s="0" t="s">
-        <x:v>76</x:v>
+        <x:v>19</x:v>
       </x:c>
       <x:c r="J47" s="0" t="s">
-        <x:v>77</x:v>
+        <x:v>20</x:v>
       </x:c>
       <x:c r="K47" s="0" t="s">
         <x:v>21</x:v>
       </x:c>
       <x:c r="L47" s="0">
-        <x:v>10</x:v>
+        <x:v>372</x:v>
       </x:c>
     </x:row>
     <x:row r="48" spans="1:15">
       <x:c r="A48" s="0" t="s">
-        <x:v>78</x:v>
+        <x:v>121</x:v>
       </x:c>
       <x:c r="B48" s="0" t="s">
-        <x:v>16</x:v>
+        <x:v>122</x:v>
       </x:c>
       <x:c r="C48" s="0" t="s">
         <x:v>17</x:v>
       </x:c>
       <x:c r="E48" s="0">
-        <x:v>67.825</x:v>
+        <x:v>78.436</x:v>
       </x:c>
       <x:c r="G48" s="0" t="s">
-        <x:v>46</x:v>
+        <x:v>32</x:v>
       </x:c>
       <x:c r="H48" s="0">
         <x:v>0</x:v>
       </x:c>
       <x:c r="L48" s="0">
         <x:v>0</x:v>
+      </x:c>
+      <x:c r="M48" s="0">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="N48" s="0" t="s">
+        <x:v>44</x:v>
+      </x:c>
+      <x:c r="O48" s="0" t="s">
+        <x:v>21</x:v>
       </x:c>
     </x:row>
     <x:row r="49" spans="1:15">
       <x:c r="A49" s="0" t="s">
-        <x:v>79</x:v>
+        <x:v>123</x:v>
       </x:c>
       <x:c r="B49" s="0" t="s">
-        <x:v>16</x:v>
+        <x:v>124</x:v>
       </x:c>
       <x:c r="C49" s="0" t="s">
         <x:v>17</x:v>
       </x:c>
       <x:c r="D49" s="0">
-        <x:v>214</x:v>
+        <x:v>473</x:v>
       </x:c>
       <x:c r="E49" s="0">
-        <x:v>80.3831</x:v>
+        <x:v>92.4321</x:v>
       </x:c>
       <x:c r="G49" s="0" t="s">
-        <x:v>24</x:v>
+        <x:v>32</x:v>
       </x:c>
       <x:c r="H49" s="0">
-        <x:v>9485.2058</x:v>
+        <x:v>10075.0989</x:v>
       </x:c>
       <x:c r="I49" s="0" t="s">
         <x:v>19</x:v>
@@ -2289,189 +2487,62 @@
         <x:v>21</x:v>
       </x:c>
       <x:c r="L49" s="0">
-        <x:v>118</x:v>
+        <x:v>109</x:v>
+      </x:c>
+      <x:c r="M49" s="0">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="N49" s="0" t="s">
+        <x:v>44</x:v>
+      </x:c>
+      <x:c r="O49" s="0" t="s">
+        <x:v>21</x:v>
       </x:c>
     </x:row>
     <x:row r="50" spans="1:15">
       <x:c r="A50" s="0" t="s">
-        <x:v>80</x:v>
+        <x:v>125</x:v>
       </x:c>
       <x:c r="B50" s="0" t="s">
-        <x:v>16</x:v>
+        <x:v>126</x:v>
       </x:c>
       <x:c r="C50" s="0" t="s">
         <x:v>17</x:v>
       </x:c>
-      <x:c r="D50" s="0">
-        <x:v>214</x:v>
-      </x:c>
       <x:c r="E50" s="0">
-        <x:v>97.239</x:v>
+        <x:v>41.0742</x:v>
       </x:c>
       <x:c r="G50" s="0" t="s">
-        <x:v>24</x:v>
+        <x:v>32</x:v>
       </x:c>
       <x:c r="H50" s="0">
-        <x:v>12446.592</x:v>
-      </x:c>
-      <x:c r="I50" s="0" t="s">
-        <x:v>19</x:v>
-      </x:c>
-      <x:c r="J50" s="0" t="s">
-        <x:v>20</x:v>
-      </x:c>
-      <x:c r="K50" s="0" t="s">
-        <x:v>21</x:v>
+        <x:v>0</x:v>
       </x:c>
       <x:c r="L50" s="0">
-        <x:v>128</x:v>
-      </x:c>
-      <x:c r="M50" s="0">
-        <x:v>4</x:v>
-      </x:c>
-      <x:c r="N50" s="0" t="s">
-        <x:v>22</x:v>
-      </x:c>
-      <x:c r="O50" s="0" t="s">
-        <x:v>21</x:v>
+        <x:v>0</x:v>
       </x:c>
     </x:row>
     <x:row r="51" spans="1:15">
       <x:c r="A51" s="0" t="s">
-        <x:v>81</x:v>
+        <x:v>127</x:v>
       </x:c>
       <x:c r="B51" s="0" t="s">
-        <x:v>16</x:v>
+        <x:v>128</x:v>
       </x:c>
       <x:c r="C51" s="0" t="s">
         <x:v>17</x:v>
       </x:c>
-      <x:c r="D51" s="0">
-        <x:v>214</x:v>
-      </x:c>
       <x:c r="E51" s="0">
-        <x:v>78.6828</x:v>
+        <x:v>7.369</x:v>
       </x:c>
       <x:c r="G51" s="0" t="s">
-        <x:v>18</x:v>
+        <x:v>47</x:v>
       </x:c>
       <x:c r="H51" s="0">
-        <x:v>8340.3768</x:v>
-      </x:c>
-      <x:c r="I51" s="0" t="s">
-        <x:v>19</x:v>
-      </x:c>
-      <x:c r="J51" s="0" t="s">
-        <x:v>20</x:v>
-      </x:c>
-      <x:c r="K51" s="0" t="s">
-        <x:v>21</x:v>
+        <x:v>0</x:v>
       </x:c>
       <x:c r="L51" s="0">
-        <x:v>106</x:v>
-      </x:c>
-      <x:c r="M51" s="0">
-        <x:v>7</x:v>
-      </x:c>
-      <x:c r="N51" s="0" t="s">
-        <x:v>22</x:v>
-      </x:c>
-      <x:c r="O51" s="0" t="s">
-        <x:v>21</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="52" spans="1:15">
-      <x:c r="A52" s="0" t="s">
-        <x:v>82</x:v>
-      </x:c>
-      <x:c r="B52" s="0" t="s">
-        <x:v>83</x:v>
-      </x:c>
-      <x:c r="C52" s="0" t="s">
-        <x:v>84</x:v>
-      </x:c>
-      <x:c r="D52" s="0">
-        <x:v>35</x:v>
-      </x:c>
-      <x:c r="E52" s="0">
-        <x:v>315</x:v>
-      </x:c>
-      <x:c r="F52" s="0" t="s">
-        <x:v>85</x:v>
-      </x:c>
-      <x:c r="G52" s="0" t="s">
-        <x:v>36</x:v>
-      </x:c>
-      <x:c r="H52" s="0">
-        <x:v>7875</x:v>
-      </x:c>
-      <x:c r="I52" s="0" t="s">
-        <x:v>56</x:v>
-      </x:c>
-      <x:c r="J52" s="0" t="s">
-        <x:v>57</x:v>
-      </x:c>
-      <x:c r="K52" s="0" t="s">
-        <x:v>86</x:v>
-      </x:c>
-      <x:c r="L52" s="0">
-        <x:v>25</x:v>
-      </x:c>
-      <x:c r="M52" s="0">
-        <x:v>9</x:v>
-      </x:c>
-      <x:c r="N52" s="0" t="s">
-        <x:v>22</x:v>
-      </x:c>
-      <x:c r="O52" s="0" t="s">
-        <x:v>21</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="53" spans="1:15">
-      <x:c r="A53" s="0" t="s">
-        <x:v>87</x:v>
-      </x:c>
-      <x:c r="B53" s="0" t="s">
-        <x:v>88</x:v>
-      </x:c>
-      <x:c r="C53" s="0" t="s">
-        <x:v>89</x:v>
-      </x:c>
-      <x:c r="D53" s="0">
-        <x:v>214</x:v>
-      </x:c>
-      <x:c r="E53" s="0">
-        <x:v>685</x:v>
-      </x:c>
-      <x:c r="F53" s="0" t="s">
-        <x:v>90</x:v>
-      </x:c>
-      <x:c r="G53" s="0" t="s">
-        <x:v>46</x:v>
-      </x:c>
-      <x:c r="H53" s="0">
-        <x:v>17125</x:v>
-      </x:c>
-      <x:c r="I53" s="0" t="s">
-        <x:v>19</x:v>
-      </x:c>
-      <x:c r="J53" s="0" t="s">
-        <x:v>20</x:v>
-      </x:c>
-      <x:c r="K53" s="0" t="s">
-        <x:v>21</x:v>
-      </x:c>
-      <x:c r="L53" s="0">
-        <x:v>25</x:v>
-      </x:c>
-      <x:c r="M53" s="0">
-        <x:v>9</x:v>
-      </x:c>
-      <x:c r="N53" s="0" t="s">
-        <x:v>22</x:v>
-      </x:c>
-      <x:c r="O53" s="0" t="s">
-        <x:v>21</x:v>
+        <x:v>0</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>